<commit_message>
[Site Web] Mise en place de diverses pages
J'ai commencer à créer plusieurs pages en rapport avec les différentes
maquettes.
</commit_message>
<xml_diff>
--- a/documents/PMP/Suivi_du_projet/Suivi_vautier.xlsx
+++ b/documents/PMP/Suivi_du_projet/Suivi_vautier.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>TACHES</t>
   </si>
@@ -68,6 +68,18 @@
   </si>
   <si>
     <t>Discussion maquette site</t>
+  </si>
+  <si>
+    <t>5.5</t>
+  </si>
+  <si>
+    <t>analyse de trame nao via wireshark Partie 2</t>
+  </si>
+  <si>
+    <t>analyse de trame nao via wireshark Partie 1</t>
+  </si>
+  <si>
+    <t>Site Internet création de quelques pages à partir des maquettes</t>
   </si>
 </sst>
 </file>
@@ -452,7 +464,7 @@
   <dimension ref="B2:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,19 +619,37 @@
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="2"/>
+      <c r="B15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="3">
+        <v>42326</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="2"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="2"/>
+      <c r="B16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="3">
+        <v>42327</v>
+      </c>
+      <c r="D16" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="B17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="3">
+        <v>42328</v>
+      </c>
+      <c r="D17" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>

</xml_diff>

<commit_message>
Correction de l'erreur de la BDD
</commit_message>
<xml_diff>
--- a/documents/PMP/Suivi_du_projet/Suivi_vautier.xlsx
+++ b/documents/PMP/Suivi_du_projet/Suivi_vautier.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>TACHES</t>
   </si>
@@ -80,6 +80,12 @@
   </si>
   <si>
     <t>Site Internet création de quelques pages à partir des maquettes</t>
+  </si>
+  <si>
+    <t>2.5</t>
+  </si>
+  <si>
+    <t>Ajout des dernières pages du site avec leurs laisons correspondantes, réorganisation des fichiers et renommage de certain. Amélioration du visuel du site</t>
   </si>
 </sst>
 </file>
@@ -464,7 +470,7 @@
   <dimension ref="B2:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,9 +658,15 @@
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+      <c r="B18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="3">
+        <v>42329</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>

</xml_diff>

<commit_message>
[Site Web] Ajout de l'affichage des commande et périphérique présent dans la BDD
</commit_message>
<xml_diff>
--- a/documents/PMP/Suivi_du_projet/Suivi_vautier.xlsx
+++ b/documents/PMP/Suivi_du_projet/Suivi_vautier.xlsx
@@ -15,12 +15,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$B$2:$D$15</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$K$32</definedName>
   </definedNames>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>TACHES</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>Ajout des dernières pages du site avec leurs laisons correspondantes, réorganisation des fichiers et renommage de certain. Amélioration du visuel du site</t>
+  </si>
+  <si>
+    <t>Ajout de l'affichage des listes des commandes et périphérique depuis la BDD</t>
   </si>
 </sst>
 </file>
@@ -470,7 +473,7 @@
   <dimension ref="B2:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="F2" sqref="F2:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,9 +672,15 @@
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+      <c r="B19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="3">
+        <v>42329</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.45</v>
+      </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>

</xml_diff>

<commit_message>
[Site Web V4] amélioration du header et des listes
</commit_message>
<xml_diff>
--- a/documents/PMP/Suivi_du_projet/Suivi_vautier.xlsx
+++ b/documents/PMP/Suivi_du_projet/Suivi_vautier.xlsx
@@ -15,7 +15,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$B$2:$D$15</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$K$32</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
@@ -88,10 +88,10 @@
     <t>Ajout des dernières pages du site avec leurs laisons correspondantes, réorganisation des fichiers et renommage de certain. Amélioration du visuel du site</t>
   </si>
   <si>
-    <t>Ajout de l'affichage des listes des commandes et périphérique depuis la BDD</t>
-  </si>
-  <si>
-    <t>Ajout de la possibilité d'ajouter/supprimer des actions/périphérique via l'accès à la BDD</t>
+    <t>Réorganisation de page / Centrage de certains élément/ refactoring / amélioration des listes</t>
+  </si>
+  <si>
+    <t>amélioration du header et refacto avec un peu de gestion de connexion d'un compte</t>
   </si>
 </sst>
 </file>
@@ -476,7 +476,7 @@
   <dimension ref="B2:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,10 +679,10 @@
         <v>22</v>
       </c>
       <c r="C19" s="3">
-        <v>42329</v>
+        <v>42330</v>
       </c>
       <c r="D19" s="2">
-        <v>0.45</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
@@ -690,10 +690,10 @@
         <v>23</v>
       </c>
       <c r="C20" s="3">
-        <v>42329</v>
+        <v>42330</v>
       </c>
       <c r="D20" s="2">
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[site web ] update de fichier divers
Model et view (dossier data)
</commit_message>
<xml_diff>
--- a/documents/PMP/Suivi_du_projet/Suivi_vautier.xlsx
+++ b/documents/PMP/Suivi_du_projet/Suivi_vautier.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>TACHES</t>
   </si>
@@ -104,6 +104,15 @@
   </si>
   <si>
     <t>Ajout de la page  viewAdministrationGuide et ajout de l'affichage des pdfs et idem pour viewguide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preparation travaux a venir </t>
+  </si>
+  <si>
+    <t>partie model (dossier data) les controlleurs avec requete sql 2</t>
+  </si>
+  <si>
+    <t>partie model (dossier data) les controlleurs avec requete sql 1</t>
   </si>
 </sst>
 </file>
@@ -241,7 +250,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -276,7 +285,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -487,8 +496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,19 +762,37 @@
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+      <c r="B25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="3">
+        <v>42338</v>
+      </c>
+      <c r="D25" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
+      <c r="B26" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="3">
+        <v>42339</v>
+      </c>
+      <c r="D26" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
+      <c r="B27" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="3">
+        <v>42341</v>
+      </c>
+      <c r="D27" s="2">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>

</xml_diff>